<commit_message>
Added url where it was missing
</commit_message>
<xml_diff>
--- a/Fordításokk - Tesztesetek.xlsx
+++ b/Fordításokk - Tesztesetek.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="155">
   <si>
     <t>Oldal</t>
   </si>
@@ -637,7 +637,27 @@
 4. Ellenőrizd, hogy valóban törlődött a fordítás</t>
   </si>
   <si>
-    <t>Fordításod = "Delilah"</t>
+    <r>
+      <rPr>
+        <sz val="12.0"/>
+      </rPr>
+      <t xml:space="preserve">URL = </t>
+    </r>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <sz val="12.0"/>
+        <u/>
+      </rPr>
+      <t>http://forditasokk.probaljaki.hu/felhasznalo/forditasaim.php</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12.0"/>
+      </rPr>
+      <t xml:space="preserve"> 
+Fordításod = "Delilah"</t>
+    </r>
   </si>
   <si>
     <t>Sikeres fordítás törlés</t>
@@ -656,6 +676,28 @@
   </si>
   <si>
     <t>1. Kattints a kijelentkezés hivatkozásra</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12.0"/>
+      </rPr>
+      <t xml:space="preserve">URL = </t>
+    </r>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <sz val="12.0"/>
+        <u/>
+      </rPr>
+      <t>http://forditasokk.probaljaki.hu/felhasznalo/forditasaim.php</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12.0"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
   </si>
   <si>
     <t>Sikeres kijelentkezés</t>
@@ -2018,7 +2060,7 @@
       <c r="H15" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="I15" s="10" t="s">
+      <c r="I15" s="7" t="s">
         <v>111</v>
       </c>
       <c r="J15" s="4" t="s">
@@ -2070,9 +2112,11 @@
       <c r="H16" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="I16" s="10"/>
+      <c r="I16" s="7" t="s">
+        <v>118</v>
+      </c>
       <c r="J16" s="4" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="K16" s="3" t="s">
         <v>22</v>
@@ -31520,8 +31564,10 @@
     <hyperlink r:id="rId10" ref="I12"/>
     <hyperlink r:id="rId11" ref="I13"/>
     <hyperlink r:id="rId12" ref="I14"/>
+    <hyperlink r:id="rId13" ref="I15"/>
+    <hyperlink r:id="rId14" ref="I16"/>
   </hyperlinks>
-  <drawing r:id="rId13"/>
+  <drawing r:id="rId15"/>
 </worksheet>
 </file>
 
@@ -31545,7 +31591,7 @@
       </c>
       <c r="R1" s="12"/>
       <c r="S1" s="11" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="X1" s="12"/>
       <c r="Y1" s="12"/>
@@ -31553,58 +31599,58 @@
     </row>
     <row r="2">
       <c r="A2" s="13" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="G2" s="13" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="H2" s="13" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="I2" s="13" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="J2" s="13" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="K2" s="13" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="L2" s="13" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="M2" s="13" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="N2" s="13" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="O2" s="13" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="P2" s="13" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="Q2" s="13" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="S2" s="14" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="X2" s="12"/>
       <c r="Y2" s="12"/>
@@ -31612,58 +31658,58 @@
     </row>
     <row r="3">
       <c r="A3" s="12" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="E3" s="15" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="F3" s="15" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="G3" s="15" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="H3" s="15" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="I3" s="15" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="J3" s="16" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="K3" s="16" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="L3" s="16" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="M3" s="16" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="N3" s="16" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="O3" s="16" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="P3" s="16" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="Q3" s="16" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="S3" s="14" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="X3" s="12"/>
       <c r="Y3" s="12"/>
@@ -31671,55 +31717,55 @@
     </row>
     <row r="4">
       <c r="A4" s="12" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="E4" s="15" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="F4" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="G4" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="H4" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="I4" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="J4" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="K4" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="L4" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="M4" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="N4" s="15" t="s">
         <v>140</v>
       </c>
-      <c r="G4" s="16" t="s">
+      <c r="O4" s="15" t="s">
         <v>140</v>
       </c>
-      <c r="H4" s="16" t="s">
+      <c r="P4" s="15" t="s">
         <v>140</v>
       </c>
-      <c r="I4" s="16" t="s">
+      <c r="Q4" s="15" t="s">
         <v>140</v>
-      </c>
-      <c r="J4" s="16" t="s">
-        <v>140</v>
-      </c>
-      <c r="K4" s="16" t="s">
-        <v>140</v>
-      </c>
-      <c r="L4" s="16" t="s">
-        <v>140</v>
-      </c>
-      <c r="M4" s="16" t="s">
-        <v>140</v>
-      </c>
-      <c r="N4" s="15" t="s">
-        <v>139</v>
-      </c>
-      <c r="O4" s="15" t="s">
-        <v>139</v>
-      </c>
-      <c r="P4" s="15" t="s">
-        <v>139</v>
-      </c>
-      <c r="Q4" s="15" t="s">
-        <v>139</v>
       </c>
       <c r="S4" s="17"/>
       <c r="X4" s="12"/>
@@ -31728,55 +31774,55 @@
     </row>
     <row r="5">
       <c r="A5" s="12" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D5" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="E5" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="F5" s="15" t="s">
         <v>140</v>
       </c>
-      <c r="E5" s="16" t="s">
+      <c r="G5" s="15" t="s">
         <v>140</v>
       </c>
-      <c r="F5" s="15" t="s">
-        <v>139</v>
+      <c r="H5" s="16" t="s">
+        <v>141</v>
       </c>
-      <c r="G5" s="15" t="s">
-        <v>139</v>
+      <c r="I5" s="16" t="s">
+        <v>141</v>
       </c>
-      <c r="H5" s="16" t="s">
+      <c r="J5" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="K5" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="L5" s="15" t="s">
         <v>140</v>
       </c>
-      <c r="I5" s="16" t="s">
+      <c r="M5" s="15" t="s">
         <v>140</v>
       </c>
-      <c r="J5" s="16" t="s">
+      <c r="N5" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="O5" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="P5" s="15" t="s">
         <v>140</v>
       </c>
-      <c r="K5" s="16" t="s">
+      <c r="Q5" s="15" t="s">
         <v>140</v>
-      </c>
-      <c r="L5" s="15" t="s">
-        <v>139</v>
-      </c>
-      <c r="M5" s="15" t="s">
-        <v>139</v>
-      </c>
-      <c r="N5" s="16" t="s">
-        <v>140</v>
-      </c>
-      <c r="O5" s="16" t="s">
-        <v>140</v>
-      </c>
-      <c r="P5" s="15" t="s">
-        <v>139</v>
-      </c>
-      <c r="Q5" s="15" t="s">
-        <v>139</v>
       </c>
       <c r="S5" s="17"/>
       <c r="X5" s="12"/>
@@ -31785,55 +31831,55 @@
     </row>
     <row r="6">
       <c r="A6" s="12" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C6" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="D6" s="15" t="s">
         <v>140</v>
       </c>
-      <c r="D6" s="15" t="s">
-        <v>139</v>
+      <c r="E6" s="16" t="s">
+        <v>141</v>
       </c>
-      <c r="E6" s="16" t="s">
+      <c r="F6" s="15" t="s">
         <v>140</v>
       </c>
-      <c r="F6" s="15" t="s">
-        <v>139</v>
+      <c r="G6" s="16" t="s">
+        <v>141</v>
       </c>
-      <c r="G6" s="16" t="s">
+      <c r="H6" s="15" t="s">
         <v>140</v>
       </c>
-      <c r="H6" s="15" t="s">
-        <v>139</v>
+      <c r="I6" s="16" t="s">
+        <v>141</v>
       </c>
-      <c r="I6" s="16" t="s">
+      <c r="J6" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="K6" s="15" t="s">
         <v>140</v>
       </c>
-      <c r="J6" s="16" t="s">
+      <c r="L6" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="M6" s="15" t="s">
         <v>140</v>
       </c>
-      <c r="K6" s="15" t="s">
-        <v>139</v>
+      <c r="N6" s="16" t="s">
+        <v>141</v>
       </c>
-      <c r="L6" s="16" t="s">
+      <c r="O6" s="15" t="s">
         <v>140</v>
       </c>
-      <c r="M6" s="15" t="s">
-        <v>139</v>
-      </c>
-      <c r="N6" s="16" t="s">
-        <v>140</v>
-      </c>
-      <c r="O6" s="15" t="s">
-        <v>139</v>
-      </c>
       <c r="P6" s="16" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="Q6" s="15" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="S6" s="17"/>
       <c r="X6" s="12"/>
@@ -31842,7 +31888,7 @@
     </row>
     <row r="7">
       <c r="A7" s="18" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B7" s="19"/>
       <c r="C7" s="19"/>
@@ -31870,7 +31916,7 @@
         <v>24</v>
       </c>
       <c r="B8" s="20" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C8" s="12"/>
       <c r="D8" s="12"/>
@@ -31894,7 +31940,7 @@
     </row>
     <row r="9">
       <c r="A9" s="12" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B9" s="12"/>
       <c r="C9" s="12"/>
@@ -31905,28 +31951,28 @@
       <c r="H9" s="12"/>
       <c r="I9" s="12"/>
       <c r="J9" s="20" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="K9" s="20" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="L9" s="20" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="M9" s="20" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="N9" s="20" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="O9" s="20" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="P9" s="20" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="Q9" s="20" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="S9" s="17"/>
       <c r="X9" s="12"/>
@@ -31935,35 +31981,35 @@
     </row>
     <row r="10">
       <c r="A10" s="12" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B10" s="12"/>
       <c r="C10" s="12"/>
       <c r="D10" s="12"/>
       <c r="E10" s="12"/>
       <c r="F10" s="20" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="G10" s="20" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="H10" s="20" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="I10" s="20" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="J10" s="20" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="K10" s="20" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="L10" s="20" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="M10" s="20" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="N10" s="12"/>
       <c r="O10" s="12"/>
@@ -31976,34 +32022,34 @@
     </row>
     <row r="11">
       <c r="A11" s="12" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B11" s="12"/>
       <c r="C11" s="12"/>
       <c r="D11" s="20" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="E11" s="20" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="F11" s="12"/>
       <c r="G11" s="12"/>
       <c r="H11" s="20" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="I11" s="20" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="J11" s="20" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="K11" s="20" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="L11" s="12"/>
       <c r="M11" s="12"/>
       <c r="N11" s="20" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="O11" s="12"/>
       <c r="P11" s="12"/>
@@ -32015,38 +32061,38 @@
     </row>
     <row r="12">
       <c r="A12" s="12" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B12" s="12"/>
       <c r="C12" s="20" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D12" s="12"/>
       <c r="E12" s="20" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="F12" s="12"/>
       <c r="G12" s="20" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="H12" s="12"/>
       <c r="I12" s="20" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="J12" s="20" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="K12" s="12"/>
       <c r="L12" s="20" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="M12" s="12"/>
       <c r="N12" s="20" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="O12" s="12"/>
       <c r="P12" s="20" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="Q12" s="12"/>
       <c r="S12" s="17"/>
@@ -32121,31 +32167,31 @@
     </row>
     <row r="16">
       <c r="A16" s="13" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D16" s="13" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E16" s="13" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="F16" s="13" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="G16" s="13" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="H16" s="13" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="I16" s="13" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="J16" s="12"/>
       <c r="K16" s="12"/>
@@ -32162,31 +32208,31 @@
     </row>
     <row r="17">
       <c r="A17" s="12" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D17" s="15" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="E17" s="15" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="F17" s="16" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="G17" s="16" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="H17" s="16" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="I17" s="16" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="K17" s="12"/>
       <c r="L17" s="12"/>
@@ -32202,31 +32248,31 @@
     </row>
     <row r="18">
       <c r="A18" s="12" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C18" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="D18" s="15" t="s">
         <v>140</v>
       </c>
-      <c r="D18" s="15" t="s">
-        <v>139</v>
+      <c r="E18" s="16" t="s">
+        <v>141</v>
       </c>
-      <c r="E18" s="16" t="s">
+      <c r="F18" s="15" t="s">
         <v>140</v>
       </c>
-      <c r="F18" s="15" t="s">
-        <v>139</v>
+      <c r="G18" s="16" t="s">
+        <v>141</v>
       </c>
-      <c r="G18" s="16" t="s">
+      <c r="H18" s="15" t="s">
         <v>140</v>
       </c>
-      <c r="H18" s="15" t="s">
-        <v>139</v>
-      </c>
       <c r="I18" s="16" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="K18" s="12"/>
       <c r="L18" s="12"/>
@@ -32242,31 +32288,31 @@
     </row>
     <row r="19">
       <c r="A19" s="21" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B19" s="22" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C19" s="22" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D19" s="23" t="s">
+        <v>141</v>
+      </c>
+      <c r="E19" s="24" t="s">
+        <v>141</v>
+      </c>
+      <c r="F19" s="15" t="s">
         <v>140</v>
       </c>
-      <c r="E19" s="24" t="s">
+      <c r="G19" s="15" t="s">
         <v>140</v>
       </c>
-      <c r="F19" s="15" t="s">
-        <v>139</v>
-      </c>
-      <c r="G19" s="15" t="s">
-        <v>139</v>
-      </c>
       <c r="H19" s="16" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="I19" s="25" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="K19" s="26"/>
       <c r="L19" s="26"/>
@@ -32286,7 +32332,7 @@
     </row>
     <row r="20">
       <c r="A20" s="18" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B20" s="19"/>
       <c r="C20" s="19"/>
@@ -32311,10 +32357,10 @@
     </row>
     <row r="21">
       <c r="A21" s="12" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B21" s="20" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C21" s="12"/>
       <c r="D21" s="12"/>
@@ -32338,29 +32384,29 @@
     </row>
     <row r="22">
       <c r="A22" s="12" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B22" s="12"/>
       <c r="C22" s="20" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D22" s="20" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="E22" s="20" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="F22" s="20" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="G22" s="20" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="H22" s="20" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="I22" s="20" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="J22" s="12"/>
       <c r="K22" s="12"/>

</xml_diff>